<commit_message>
added 50 more patients
</commit_message>
<xml_diff>
--- a/fpar/patient_list_01.xlsx
+++ b/fpar/patient_list_01.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="402">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -926,6 +926,306 @@
   </si>
   <si>
     <t xml:space="preserve">ACEVEDO,Kimberly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARRISON,Janet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13702</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STEIN,Janet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13737</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARSONS,Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BASS,Megan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARDNER,Stephen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCCLAIN,Hannah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BULLOCK,Debra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVILA,Brittany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13949</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BALL,Nicholas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REYNOLDS,Kelly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENDER,Amy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WATKINS,Rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DILLON,Betty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHANG,Betty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIGUEROA,Debra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLETCHER,Rachel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCCULLOUGH,Heather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHERMAN,Evelyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARREN,Nicole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEON,Andrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLINE,Lauren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COCHRAN,Virginia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HENSLEY,Beverly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14482</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HATFIELD,Anna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14518</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEYERS,Marilyn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANDALL,Amber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14589</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FINLEY,Olivia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLON,Laura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUELLER,Dorothy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANNON,Megan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENTON,Marie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARREN,Olivia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BISHOP,Kathryn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FISCHER,Jean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWEENEY,Amanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARTLETT,Dorothy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14944</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLARKE,Martha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUCKER,Linda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLSEN,Sandra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPSON,Sara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLYNN,Janet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLAKE,Melissa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEMENTS,Stephen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURTIS,Victoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOORE,Sarah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANDOLPH,Andrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PETTY,Cheryl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FISCHER,Carol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MITCHELL,Victoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRADFORD,Steven</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1341,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B127" activeCellId="0" sqref="A:B"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A152" activeCellId="0" sqref="A152:B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2262,6 +2562,406 @@
         <v>301</v>
       </c>
     </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B189" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" s="0" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B198" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>401</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>